<commit_message>
excel products ready to import to shop, only needs fixes in backend to be properly displayed in front.
</commit_message>
<xml_diff>
--- a/djv-product/src/main/resources/excel/products.xlsx
+++ b/djv-product/src/main/resources/excel/products.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\margi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\margi\Desktop\Unik Stuff\PSK\dejavu-online-shop\djv-product\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1880" uniqueCount="455">
   <si>
     <t>Title</t>
   </si>
@@ -1382,6 +1382,9 @@
   </si>
   <si>
     <t>0.32 ounces</t>
+  </si>
+  <si>
+    <t>category/path/to/product</t>
   </si>
 </sst>
 </file>
@@ -1881,7 +1884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R584"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A562" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A382" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I585" sqref="I585"/>
     </sheetView>
   </sheetViews>
@@ -11606,42 +11609,192 @@
     </row>
   </sheetData>
   <mergeCells count="240">
-    <mergeCell ref="A572:A581"/>
-    <mergeCell ref="B572:B581"/>
-    <mergeCell ref="C572:C581"/>
-    <mergeCell ref="D572:D581"/>
-    <mergeCell ref="E572:E581"/>
-    <mergeCell ref="F572:F581"/>
-    <mergeCell ref="A582:A584"/>
-    <mergeCell ref="B582:B584"/>
-    <mergeCell ref="C582:C584"/>
-    <mergeCell ref="D582:D584"/>
-    <mergeCell ref="E582:E584"/>
-    <mergeCell ref="F582:F584"/>
-    <mergeCell ref="F2:F16"/>
-    <mergeCell ref="A17:A35"/>
-    <mergeCell ref="B17:B35"/>
-    <mergeCell ref="C17:C35"/>
-    <mergeCell ref="D17:D35"/>
-    <mergeCell ref="E17:E35"/>
-    <mergeCell ref="F17:F35"/>
-    <mergeCell ref="A2:A16"/>
-    <mergeCell ref="B2:B16"/>
-    <mergeCell ref="C2:C16"/>
-    <mergeCell ref="D2:D16"/>
-    <mergeCell ref="E2:E16"/>
-    <mergeCell ref="F36:F50"/>
-    <mergeCell ref="A51:A67"/>
-    <mergeCell ref="B51:B67"/>
-    <mergeCell ref="C51:C67"/>
-    <mergeCell ref="D51:D67"/>
-    <mergeCell ref="E51:E67"/>
-    <mergeCell ref="F51:F67"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="B36:B50"/>
-    <mergeCell ref="C36:C50"/>
-    <mergeCell ref="D36:D50"/>
-    <mergeCell ref="E36:E50"/>
+    <mergeCell ref="A542:A559"/>
+    <mergeCell ref="B542:B559"/>
+    <mergeCell ref="C542:C559"/>
+    <mergeCell ref="D542:D559"/>
+    <mergeCell ref="E542:E559"/>
+    <mergeCell ref="F542:F559"/>
+    <mergeCell ref="A560:A571"/>
+    <mergeCell ref="B560:B571"/>
+    <mergeCell ref="C560:C571"/>
+    <mergeCell ref="D560:D571"/>
+    <mergeCell ref="E560:E571"/>
+    <mergeCell ref="F560:F571"/>
+    <mergeCell ref="A516:A529"/>
+    <mergeCell ref="B516:B529"/>
+    <mergeCell ref="C516:C529"/>
+    <mergeCell ref="D516:D529"/>
+    <mergeCell ref="E516:E529"/>
+    <mergeCell ref="F516:F529"/>
+    <mergeCell ref="A530:A541"/>
+    <mergeCell ref="B530:B541"/>
+    <mergeCell ref="C530:C541"/>
+    <mergeCell ref="D530:D541"/>
+    <mergeCell ref="E530:E541"/>
+    <mergeCell ref="F530:F541"/>
+    <mergeCell ref="F512:F515"/>
+    <mergeCell ref="A512:A515"/>
+    <mergeCell ref="B512:B515"/>
+    <mergeCell ref="C512:C515"/>
+    <mergeCell ref="D512:D515"/>
+    <mergeCell ref="E512:E515"/>
+    <mergeCell ref="F481:F496"/>
+    <mergeCell ref="A497:A511"/>
+    <mergeCell ref="B497:B511"/>
+    <mergeCell ref="C497:C511"/>
+    <mergeCell ref="D497:D511"/>
+    <mergeCell ref="E497:E511"/>
+    <mergeCell ref="F497:F511"/>
+    <mergeCell ref="A481:A496"/>
+    <mergeCell ref="B481:B496"/>
+    <mergeCell ref="C481:C496"/>
+    <mergeCell ref="D481:D496"/>
+    <mergeCell ref="E481:E496"/>
+    <mergeCell ref="F451:F464"/>
+    <mergeCell ref="A465:A480"/>
+    <mergeCell ref="B465:B480"/>
+    <mergeCell ref="C465:C480"/>
+    <mergeCell ref="D465:D480"/>
+    <mergeCell ref="E465:E480"/>
+    <mergeCell ref="F465:F480"/>
+    <mergeCell ref="A451:A464"/>
+    <mergeCell ref="B451:B464"/>
+    <mergeCell ref="C451:C464"/>
+    <mergeCell ref="D451:D464"/>
+    <mergeCell ref="E451:E464"/>
+    <mergeCell ref="F422:F436"/>
+    <mergeCell ref="A437:A450"/>
+    <mergeCell ref="B437:B450"/>
+    <mergeCell ref="C437:C450"/>
+    <mergeCell ref="D437:D450"/>
+    <mergeCell ref="E437:E450"/>
+    <mergeCell ref="F437:F450"/>
+    <mergeCell ref="A422:A436"/>
+    <mergeCell ref="B422:B436"/>
+    <mergeCell ref="C422:C436"/>
+    <mergeCell ref="D422:D436"/>
+    <mergeCell ref="E422:E436"/>
+    <mergeCell ref="F391:F407"/>
+    <mergeCell ref="A408:A421"/>
+    <mergeCell ref="B408:B421"/>
+    <mergeCell ref="C408:C421"/>
+    <mergeCell ref="D408:D421"/>
+    <mergeCell ref="E408:E421"/>
+    <mergeCell ref="F408:F421"/>
+    <mergeCell ref="A391:A407"/>
+    <mergeCell ref="B391:B407"/>
+    <mergeCell ref="C391:C407"/>
+    <mergeCell ref="D391:D407"/>
+    <mergeCell ref="E391:E407"/>
+    <mergeCell ref="F358:F373"/>
+    <mergeCell ref="A374:A390"/>
+    <mergeCell ref="B374:B390"/>
+    <mergeCell ref="C374:C390"/>
+    <mergeCell ref="D374:D390"/>
+    <mergeCell ref="E374:E390"/>
+    <mergeCell ref="F374:F390"/>
+    <mergeCell ref="A358:A373"/>
+    <mergeCell ref="B358:B373"/>
+    <mergeCell ref="C358:C373"/>
+    <mergeCell ref="D358:D373"/>
+    <mergeCell ref="E358:E373"/>
+    <mergeCell ref="F325:F341"/>
+    <mergeCell ref="A342:A357"/>
+    <mergeCell ref="B342:B357"/>
+    <mergeCell ref="C342:C357"/>
+    <mergeCell ref="D342:D357"/>
+    <mergeCell ref="E342:E357"/>
+    <mergeCell ref="F342:F357"/>
+    <mergeCell ref="A325:A341"/>
+    <mergeCell ref="B325:B341"/>
+    <mergeCell ref="C325:C341"/>
+    <mergeCell ref="D325:D341"/>
+    <mergeCell ref="E325:E341"/>
+    <mergeCell ref="F304:F307"/>
+    <mergeCell ref="A308:A324"/>
+    <mergeCell ref="B308:B324"/>
+    <mergeCell ref="C308:C324"/>
+    <mergeCell ref="D308:D324"/>
+    <mergeCell ref="E308:E324"/>
+    <mergeCell ref="F308:F324"/>
+    <mergeCell ref="A304:A307"/>
+    <mergeCell ref="B304:B307"/>
+    <mergeCell ref="C304:C307"/>
+    <mergeCell ref="D304:D307"/>
+    <mergeCell ref="E304:E307"/>
+    <mergeCell ref="F271:F287"/>
+    <mergeCell ref="A288:A303"/>
+    <mergeCell ref="B288:B303"/>
+    <mergeCell ref="C288:C303"/>
+    <mergeCell ref="D288:D303"/>
+    <mergeCell ref="E288:E303"/>
+    <mergeCell ref="F288:F303"/>
+    <mergeCell ref="A271:A287"/>
+    <mergeCell ref="B271:B287"/>
+    <mergeCell ref="C271:C287"/>
+    <mergeCell ref="D271:D287"/>
+    <mergeCell ref="E271:E287"/>
+    <mergeCell ref="F238:F254"/>
+    <mergeCell ref="A255:A270"/>
+    <mergeCell ref="B255:B270"/>
+    <mergeCell ref="C255:C270"/>
+    <mergeCell ref="D255:D270"/>
+    <mergeCell ref="E255:E270"/>
+    <mergeCell ref="F255:F270"/>
+    <mergeCell ref="A238:A254"/>
+    <mergeCell ref="B238:B254"/>
+    <mergeCell ref="C238:C254"/>
+    <mergeCell ref="D238:D254"/>
+    <mergeCell ref="E238:E254"/>
+    <mergeCell ref="F204:F220"/>
+    <mergeCell ref="A221:A237"/>
+    <mergeCell ref="B221:B237"/>
+    <mergeCell ref="C221:C237"/>
+    <mergeCell ref="D221:D237"/>
+    <mergeCell ref="E221:E237"/>
+    <mergeCell ref="F221:F237"/>
+    <mergeCell ref="A204:A220"/>
+    <mergeCell ref="B204:B220"/>
+    <mergeCell ref="C204:C220"/>
+    <mergeCell ref="D204:D220"/>
+    <mergeCell ref="E204:E220"/>
+    <mergeCell ref="F170:F186"/>
+    <mergeCell ref="A187:A203"/>
+    <mergeCell ref="B187:B203"/>
+    <mergeCell ref="C187:C203"/>
+    <mergeCell ref="D187:D203"/>
+    <mergeCell ref="E187:E203"/>
+    <mergeCell ref="F187:F203"/>
+    <mergeCell ref="A170:A186"/>
+    <mergeCell ref="B170:B186"/>
+    <mergeCell ref="C170:C186"/>
+    <mergeCell ref="D170:D186"/>
+    <mergeCell ref="E170:E186"/>
+    <mergeCell ref="F138:F153"/>
+    <mergeCell ref="A154:A169"/>
+    <mergeCell ref="B154:B169"/>
+    <mergeCell ref="C154:C169"/>
+    <mergeCell ref="D154:D169"/>
+    <mergeCell ref="E154:E169"/>
+    <mergeCell ref="F154:F169"/>
+    <mergeCell ref="A138:A153"/>
+    <mergeCell ref="B138:B153"/>
+    <mergeCell ref="C138:C153"/>
+    <mergeCell ref="D138:D153"/>
+    <mergeCell ref="E138:E153"/>
+    <mergeCell ref="F107:F121"/>
+    <mergeCell ref="A122:A137"/>
+    <mergeCell ref="B122:B137"/>
+    <mergeCell ref="C122:C137"/>
+    <mergeCell ref="D122:D137"/>
+    <mergeCell ref="E122:E137"/>
+    <mergeCell ref="F122:F137"/>
+    <mergeCell ref="A107:A121"/>
+    <mergeCell ref="B107:B121"/>
+    <mergeCell ref="C107:C121"/>
+    <mergeCell ref="D107:D121"/>
+    <mergeCell ref="E107:E121"/>
     <mergeCell ref="F93:F106"/>
     <mergeCell ref="A93:A106"/>
     <mergeCell ref="B93:B106"/>
@@ -11660,192 +11813,42 @@
     <mergeCell ref="C68:C84"/>
     <mergeCell ref="D68:D84"/>
     <mergeCell ref="E68:E84"/>
-    <mergeCell ref="F107:F121"/>
-    <mergeCell ref="A122:A137"/>
-    <mergeCell ref="B122:B137"/>
-    <mergeCell ref="C122:C137"/>
-    <mergeCell ref="D122:D137"/>
-    <mergeCell ref="E122:E137"/>
-    <mergeCell ref="F122:F137"/>
-    <mergeCell ref="A107:A121"/>
-    <mergeCell ref="B107:B121"/>
-    <mergeCell ref="C107:C121"/>
-    <mergeCell ref="D107:D121"/>
-    <mergeCell ref="E107:E121"/>
-    <mergeCell ref="F138:F153"/>
-    <mergeCell ref="A154:A169"/>
-    <mergeCell ref="B154:B169"/>
-    <mergeCell ref="C154:C169"/>
-    <mergeCell ref="D154:D169"/>
-    <mergeCell ref="E154:E169"/>
-    <mergeCell ref="F154:F169"/>
-    <mergeCell ref="A138:A153"/>
-    <mergeCell ref="B138:B153"/>
-    <mergeCell ref="C138:C153"/>
-    <mergeCell ref="D138:D153"/>
-    <mergeCell ref="E138:E153"/>
-    <mergeCell ref="F170:F186"/>
-    <mergeCell ref="A187:A203"/>
-    <mergeCell ref="B187:B203"/>
-    <mergeCell ref="C187:C203"/>
-    <mergeCell ref="D187:D203"/>
-    <mergeCell ref="E187:E203"/>
-    <mergeCell ref="F187:F203"/>
-    <mergeCell ref="A170:A186"/>
-    <mergeCell ref="B170:B186"/>
-    <mergeCell ref="C170:C186"/>
-    <mergeCell ref="D170:D186"/>
-    <mergeCell ref="E170:E186"/>
-    <mergeCell ref="F204:F220"/>
-    <mergeCell ref="A221:A237"/>
-    <mergeCell ref="B221:B237"/>
-    <mergeCell ref="C221:C237"/>
-    <mergeCell ref="D221:D237"/>
-    <mergeCell ref="E221:E237"/>
-    <mergeCell ref="F221:F237"/>
-    <mergeCell ref="A204:A220"/>
-    <mergeCell ref="B204:B220"/>
-    <mergeCell ref="C204:C220"/>
-    <mergeCell ref="D204:D220"/>
-    <mergeCell ref="E204:E220"/>
-    <mergeCell ref="F238:F254"/>
-    <mergeCell ref="A255:A270"/>
-    <mergeCell ref="B255:B270"/>
-    <mergeCell ref="C255:C270"/>
-    <mergeCell ref="D255:D270"/>
-    <mergeCell ref="E255:E270"/>
-    <mergeCell ref="F255:F270"/>
-    <mergeCell ref="A238:A254"/>
-    <mergeCell ref="B238:B254"/>
-    <mergeCell ref="C238:C254"/>
-    <mergeCell ref="D238:D254"/>
-    <mergeCell ref="E238:E254"/>
-    <mergeCell ref="F271:F287"/>
-    <mergeCell ref="A288:A303"/>
-    <mergeCell ref="B288:B303"/>
-    <mergeCell ref="C288:C303"/>
-    <mergeCell ref="D288:D303"/>
-    <mergeCell ref="E288:E303"/>
-    <mergeCell ref="F288:F303"/>
-    <mergeCell ref="A271:A287"/>
-    <mergeCell ref="B271:B287"/>
-    <mergeCell ref="C271:C287"/>
-    <mergeCell ref="D271:D287"/>
-    <mergeCell ref="E271:E287"/>
-    <mergeCell ref="F304:F307"/>
-    <mergeCell ref="A308:A324"/>
-    <mergeCell ref="B308:B324"/>
-    <mergeCell ref="C308:C324"/>
-    <mergeCell ref="D308:D324"/>
-    <mergeCell ref="E308:E324"/>
-    <mergeCell ref="F308:F324"/>
-    <mergeCell ref="A304:A307"/>
-    <mergeCell ref="B304:B307"/>
-    <mergeCell ref="C304:C307"/>
-    <mergeCell ref="D304:D307"/>
-    <mergeCell ref="E304:E307"/>
-    <mergeCell ref="F325:F341"/>
-    <mergeCell ref="A342:A357"/>
-    <mergeCell ref="B342:B357"/>
-    <mergeCell ref="C342:C357"/>
-    <mergeCell ref="D342:D357"/>
-    <mergeCell ref="E342:E357"/>
-    <mergeCell ref="F342:F357"/>
-    <mergeCell ref="A325:A341"/>
-    <mergeCell ref="B325:B341"/>
-    <mergeCell ref="C325:C341"/>
-    <mergeCell ref="D325:D341"/>
-    <mergeCell ref="E325:E341"/>
-    <mergeCell ref="F358:F373"/>
-    <mergeCell ref="A374:A390"/>
-    <mergeCell ref="B374:B390"/>
-    <mergeCell ref="C374:C390"/>
-    <mergeCell ref="D374:D390"/>
-    <mergeCell ref="E374:E390"/>
-    <mergeCell ref="F374:F390"/>
-    <mergeCell ref="A358:A373"/>
-    <mergeCell ref="B358:B373"/>
-    <mergeCell ref="C358:C373"/>
-    <mergeCell ref="D358:D373"/>
-    <mergeCell ref="E358:E373"/>
-    <mergeCell ref="F391:F407"/>
-    <mergeCell ref="A408:A421"/>
-    <mergeCell ref="B408:B421"/>
-    <mergeCell ref="C408:C421"/>
-    <mergeCell ref="D408:D421"/>
-    <mergeCell ref="E408:E421"/>
-    <mergeCell ref="F408:F421"/>
-    <mergeCell ref="A391:A407"/>
-    <mergeCell ref="B391:B407"/>
-    <mergeCell ref="C391:C407"/>
-    <mergeCell ref="D391:D407"/>
-    <mergeCell ref="E391:E407"/>
-    <mergeCell ref="F422:F436"/>
-    <mergeCell ref="A437:A450"/>
-    <mergeCell ref="B437:B450"/>
-    <mergeCell ref="C437:C450"/>
-    <mergeCell ref="D437:D450"/>
-    <mergeCell ref="E437:E450"/>
-    <mergeCell ref="F437:F450"/>
-    <mergeCell ref="A422:A436"/>
-    <mergeCell ref="B422:B436"/>
-    <mergeCell ref="C422:C436"/>
-    <mergeCell ref="D422:D436"/>
-    <mergeCell ref="E422:E436"/>
-    <mergeCell ref="F451:F464"/>
-    <mergeCell ref="A465:A480"/>
-    <mergeCell ref="B465:B480"/>
-    <mergeCell ref="C465:C480"/>
-    <mergeCell ref="D465:D480"/>
-    <mergeCell ref="E465:E480"/>
-    <mergeCell ref="F465:F480"/>
-    <mergeCell ref="A451:A464"/>
-    <mergeCell ref="B451:B464"/>
-    <mergeCell ref="C451:C464"/>
-    <mergeCell ref="D451:D464"/>
-    <mergeCell ref="E451:E464"/>
-    <mergeCell ref="F512:F515"/>
-    <mergeCell ref="A512:A515"/>
-    <mergeCell ref="B512:B515"/>
-    <mergeCell ref="C512:C515"/>
-    <mergeCell ref="D512:D515"/>
-    <mergeCell ref="E512:E515"/>
-    <mergeCell ref="F481:F496"/>
-    <mergeCell ref="A497:A511"/>
-    <mergeCell ref="B497:B511"/>
-    <mergeCell ref="C497:C511"/>
-    <mergeCell ref="D497:D511"/>
-    <mergeCell ref="E497:E511"/>
-    <mergeCell ref="F497:F511"/>
-    <mergeCell ref="A481:A496"/>
-    <mergeCell ref="B481:B496"/>
-    <mergeCell ref="C481:C496"/>
-    <mergeCell ref="D481:D496"/>
-    <mergeCell ref="E481:E496"/>
-    <mergeCell ref="A516:A529"/>
-    <mergeCell ref="B516:B529"/>
-    <mergeCell ref="C516:C529"/>
-    <mergeCell ref="D516:D529"/>
-    <mergeCell ref="E516:E529"/>
-    <mergeCell ref="F516:F529"/>
-    <mergeCell ref="A530:A541"/>
-    <mergeCell ref="B530:B541"/>
-    <mergeCell ref="C530:C541"/>
-    <mergeCell ref="D530:D541"/>
-    <mergeCell ref="E530:E541"/>
-    <mergeCell ref="F530:F541"/>
-    <mergeCell ref="A542:A559"/>
-    <mergeCell ref="B542:B559"/>
-    <mergeCell ref="C542:C559"/>
-    <mergeCell ref="D542:D559"/>
-    <mergeCell ref="E542:E559"/>
-    <mergeCell ref="F542:F559"/>
-    <mergeCell ref="A560:A571"/>
-    <mergeCell ref="B560:B571"/>
-    <mergeCell ref="C560:C571"/>
-    <mergeCell ref="D560:D571"/>
-    <mergeCell ref="E560:E571"/>
-    <mergeCell ref="F560:F571"/>
+    <mergeCell ref="F36:F50"/>
+    <mergeCell ref="A51:A67"/>
+    <mergeCell ref="B51:B67"/>
+    <mergeCell ref="C51:C67"/>
+    <mergeCell ref="D51:D67"/>
+    <mergeCell ref="E51:E67"/>
+    <mergeCell ref="F51:F67"/>
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="B36:B50"/>
+    <mergeCell ref="C36:C50"/>
+    <mergeCell ref="D36:D50"/>
+    <mergeCell ref="E36:E50"/>
+    <mergeCell ref="F2:F16"/>
+    <mergeCell ref="A17:A35"/>
+    <mergeCell ref="B17:B35"/>
+    <mergeCell ref="C17:C35"/>
+    <mergeCell ref="D17:D35"/>
+    <mergeCell ref="E17:E35"/>
+    <mergeCell ref="F17:F35"/>
+    <mergeCell ref="A2:A16"/>
+    <mergeCell ref="B2:B16"/>
+    <mergeCell ref="C2:C16"/>
+    <mergeCell ref="D2:D16"/>
+    <mergeCell ref="E2:E16"/>
+    <mergeCell ref="A572:A581"/>
+    <mergeCell ref="B572:B581"/>
+    <mergeCell ref="C572:C581"/>
+    <mergeCell ref="D572:D581"/>
+    <mergeCell ref="E572:E581"/>
+    <mergeCell ref="F572:F581"/>
+    <mergeCell ref="A582:A584"/>
+    <mergeCell ref="B582:B584"/>
+    <mergeCell ref="C582:C584"/>
+    <mergeCell ref="D582:D584"/>
+    <mergeCell ref="E582:E584"/>
+    <mergeCell ref="F582:F584"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -11856,8 +11859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11880,7 +11883,7 @@
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
       <c r="F1" s="15" t="s">
-        <v>6</v>
+        <v>454</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>7</v>

</xml_diff>